<commit_message>
Updated benchmark for Linux as well.
</commit_message>
<xml_diff>
--- a/benchmark/results.v2.1.xlsx
+++ b/benchmark/results.v2.1.xlsx
@@ -16,12 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Compiler</t>
-  </si>
-  <si>
-    <t>xcode82</t>
   </si>
   <si>
     <t>gcc74-noexcept</t>
@@ -163,7 +160,7 @@
             <c:strRef>
               <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>gcc74-noexcept</c:v>
                 </c:pt>
@@ -184,30 +181,27 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>msvc1916-ltcg</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>xcode82</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:f>Sheet1!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>87.501360000000005</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>82.424570000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>87.8964</c:v>
+                  <c:v>82.707740000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>101.42652</c:v>
+                  <c:v>91.374139999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.8998</c:v>
+                  <c:v>80.194599999999994</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>96.921149999999997</c:v>
@@ -217,9 +211,6 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>96.569659999999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>86.842960000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -248,7 +239,7 @@
             <c:strRef>
               <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>gcc74-noexcept</c:v>
                 </c:pt>
@@ -269,30 +260,27 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>msvc1916-ltcg</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>xcode82</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:f>Sheet1!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>94.67792</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>81.678510000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>95.204639999999998</c:v>
+                  <c:v>88.960840000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>104.35639999999999</c:v>
+                  <c:v>92.785290000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.069119999999998</c:v>
+                  <c:v>83.502340000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>110.91655</c:v>
@@ -302,9 +290,6 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>118.07134000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>93.196520000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -333,7 +318,7 @@
             <c:strRef>
               <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>gcc74-noexcept</c:v>
                 </c:pt>
@@ -354,42 +339,36 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>msvc1916-ltcg</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>xcode82</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$11</c:f>
+              <c:f>Sheet1!$E$2:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>91.089640000000003</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>82.764660000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90.29956</c:v>
+                  <c:v>85.397329999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>96.620199999999997</c:v>
+                  <c:v>91.785889999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.464160000000007</c:v>
+                  <c:v>90.926379999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>176.76660000000001</c:v>
+                  <c:v>129.85785000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>132.70983000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>85.29853</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>96.521439999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -419,10 +398,22 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$11</c:f>
+              <c:f>Sheet1!$H$2:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>88.50273</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82.794759999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87.292519999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>86.220759999999999</c:v>
+                </c:pt>
                 <c:pt idx="5">
                   <c:v>87.248260000000002</c:v>
                 </c:pt>
@@ -460,10 +451,22 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$11</c:f>
+              <c:f>Sheet1!$I$2:$I$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>85.55274</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>86.688599999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>89.312989999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>83.911699999999996</c:v>
+                </c:pt>
                 <c:pt idx="5">
                   <c:v>83.607500000000002</c:v>
                 </c:pt>
@@ -498,50 +501,47 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$11</c:f>
+              <c:f>Sheet1!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="1">
-                  <c:v>35030.171999999999</c:v>
+                  <c:v>41302.28213</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3801.8320399999998</c:v>
+                  <c:v>4605.8144899999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33278.30128</c:v>
+                  <c:v>42709.761350000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>27334.886299999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>25847.482609999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>21292.326799999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="173024000"/>
-        <c:axId val="173025536"/>
+        <c:axId val="104049664"/>
+        <c:axId val="104362752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="173024000"/>
+        <c:axId val="104049664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173025536"/>
+        <c:crossAx val="104362752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="173025536"/>
+        <c:axId val="104362752"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -568,7 +568,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173024000"/>
+        <c:crossAx val="104049664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -591,7 +591,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -612,7 +612,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Cost of returning error up ten stack frames on x64</a:t>
+              <a:t>Cost of traversing ten stack frames on x64</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -640,14 +640,14 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="FF0000"/>
+              <a:srgbClr val="92D050"/>
             </a:solidFill>
           </c:spPr>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>gcc74-noexcept</c:v>
                 </c:pt>
@@ -668,30 +668,27 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>msvc1916-ltcg</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>xcode82</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:f>Sheet1!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>87.501360000000005</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>82.424570000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>87.8964</c:v>
+                  <c:v>82.707740000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>101.42652</c:v>
+                  <c:v>91.374139999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.8998</c:v>
+                  <c:v>80.194599999999994</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>96.921149999999997</c:v>
@@ -701,9 +698,6 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>96.569659999999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>86.842960000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -725,14 +719,14 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="92D050"/>
+              <a:srgbClr val="00B050"/>
             </a:solidFill>
           </c:spPr>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>gcc74-noexcept</c:v>
                 </c:pt>
@@ -753,30 +747,27 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>msvc1916-ltcg</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>xcode82</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:f>Sheet1!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>94.67792</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>81.678510000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>95.204639999999998</c:v>
+                  <c:v>88.960840000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>104.35639999999999</c:v>
+                  <c:v>92.785290000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.069119999999998</c:v>
+                  <c:v>83.502340000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>110.91655</c:v>
@@ -786,9 +777,6 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>118.07134000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>93.196520000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -810,14 +798,14 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="00B050"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
           </c:spPr>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>gcc74-noexcept</c:v>
                 </c:pt>
@@ -838,42 +826,36 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>msvc1916-ltcg</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>xcode82</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$11</c:f>
+              <c:f>Sheet1!$E$2:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>91.089640000000003</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>82.764660000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90.29956</c:v>
+                  <c:v>85.397329999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>96.620199999999997</c:v>
+                  <c:v>91.785889999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.464160000000007</c:v>
+                  <c:v>90.926379999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>176.76660000000001</c:v>
+                  <c:v>129.85785000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>132.70983000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>85.29853</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>96.521439999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -884,100 +866,126 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>exception throw-catch</c:v>
+                  <c:v>success (experimental status code)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="FFFF00"/>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
             </a:solidFill>
           </c:spPr>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>gcc74-noexcept</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>gcc74</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>gcc74-lto</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>clang80</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>msvc1916-noexcept</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>msvc1916</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>msvc1916-ltcg</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>xcode82</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$11</c:f>
+              <c:f>Sheet1!$H$2:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>88.50273</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>35030.171999999999</c:v>
+                  <c:v>82.794759999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3801.8320399999998</c:v>
+                  <c:v>87.292519999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33278.30128</c:v>
+                  <c:v>86.220759999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87.248260000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27334.886299999998</c:v>
+                  <c:v>93.45993</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25847.482609999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>21292.326799999999</c:v>
+                  <c:v>93.096260000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="173073536"/>
-        <c:axId val="173075072"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>failure (experimental status code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>85.55274</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>86.688599999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>89.312989999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>83.911699999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>83.607500000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>87.351600000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>86.162400000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="119894784"/>
+        <c:axId val="184440320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="173073536"/>
+        <c:axId val="119894784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173075072"/>
+        <c:crossAx val="184440320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="173075072"/>
+        <c:axId val="184440320"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
@@ -1002,7 +1010,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173073536"/>
+        <c:crossAx val="119894784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1025,7 +1033,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1066,19 +1074,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>222300</xdr:colOff>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>38150</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>136950</xdr:rowOff>
+      <xdr:rowOff>130600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1381,10 +1389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1405,122 +1413,146 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>87.501360000000005</v>
+        <v>82.424570000000003</v>
       </c>
       <c r="D2">
-        <v>94.67792</v>
+        <v>81.678510000000003</v>
       </c>
       <c r="E2">
-        <v>91.089640000000003</v>
+        <v>82.764660000000006</v>
       </c>
       <c r="F2">
-        <v>92.176000000000002</v>
+        <v>98.672160000000005</v>
       </c>
       <c r="G2">
-        <v>99.48424</v>
+        <v>96.565849999999998</v>
+      </c>
+      <c r="H2">
+        <v>88.50273</v>
+      </c>
+      <c r="I2">
+        <v>85.55274</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>87.8964</v>
+        <v>82.707740000000001</v>
       </c>
       <c r="C3">
-        <v>35030.171999999999</v>
+        <v>41302.28213</v>
       </c>
       <c r="D3">
-        <v>95.204639999999998</v>
+        <v>88.960840000000005</v>
       </c>
       <c r="E3">
-        <v>90.29956</v>
+        <v>85.397329999999997</v>
       </c>
       <c r="F3">
-        <v>94.249960000000002</v>
+        <v>86.400289999999998</v>
       </c>
       <c r="G3">
-        <v>298.81484</v>
+        <v>481.47708999999998</v>
+      </c>
+      <c r="H3">
+        <v>82.794759999999997</v>
+      </c>
+      <c r="I3">
+        <v>86.688599999999994</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>101.42652</v>
+        <v>91.374139999999997</v>
       </c>
       <c r="C4">
-        <v>3801.8320399999998</v>
+        <v>4605.8144899999998</v>
       </c>
       <c r="D4">
-        <v>104.35639999999999</v>
+        <v>92.785290000000003</v>
       </c>
       <c r="E4">
-        <v>96.620199999999997</v>
+        <v>91.785889999999995</v>
       </c>
       <c r="F4">
-        <v>94.381640000000004</v>
+        <v>93.126189999999994</v>
       </c>
       <c r="G4">
-        <v>298.61732000000001</v>
+        <v>305.27650999999997</v>
+      </c>
+      <c r="H4">
+        <v>87.292519999999996</v>
+      </c>
+      <c r="I4">
+        <v>89.312989999999999</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>100.8998</v>
+        <v>80.194599999999994</v>
       </c>
       <c r="C5">
-        <v>33278.30128</v>
+        <v>42709.761350000001</v>
       </c>
       <c r="D5">
-        <v>90.069119999999998</v>
+        <v>83.502340000000004</v>
       </c>
       <c r="E5">
-        <v>90.464160000000007</v>
+        <v>90.926379999999995</v>
       </c>
       <c r="F5">
-        <v>96.686040000000006</v>
+        <v>93.079610000000002</v>
       </c>
       <c r="G5">
-        <v>308.09827999999999</v>
+        <v>388.19351</v>
+      </c>
+      <c r="H5">
+        <v>86.220759999999999</v>
+      </c>
+      <c r="I5">
+        <v>83.911699999999996</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>96.921149999999997</v>
@@ -1529,7 +1561,7 @@
         <v>110.91655</v>
       </c>
       <c r="E7">
-        <v>176.76660000000001</v>
+        <v>129.85785000000001</v>
       </c>
       <c r="F7">
         <v>91.225800000000007</v>
@@ -1546,7 +1578,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>82.727720000000005</v>
@@ -1575,7 +1607,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>96.569659999999999</v>
@@ -1600,29 +1632,6 @@
       </c>
       <c r="I9">
         <v>86.162400000000005</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>86.842960000000005</v>
-      </c>
-      <c r="C11">
-        <v>21292.326799999999</v>
-      </c>
-      <c r="D11">
-        <v>93.196520000000007</v>
-      </c>
-      <c r="E11">
-        <v>96.521439999999998</v>
-      </c>
-      <c r="F11">
-        <v>93.920760000000001</v>
-      </c>
-      <c r="G11">
-        <v>3139.0207599999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Specify exact CPU in benchmark.
</commit_message>
<xml_diff>
--- a/benchmark/results.v2.1.xlsx
+++ b/benchmark/results.v2.1.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="17790" windowHeight="12320"/>
+    <workbookView xWindow="240" yWindow="113" windowWidth="23168" windowHeight="12503"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Intel Skylake x64" sheetId="1" r:id="rId1"/>
+    <sheet name="Intel Silvermont x64" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Compiler</t>
   </si>
@@ -64,6 +63,24 @@
   </si>
   <si>
     <t>failure (experimental status code)</t>
+  </si>
+  <si>
+    <t>clang73</t>
+  </si>
+  <si>
+    <t>gcc73-noexcept</t>
+  </si>
+  <si>
+    <t>gcc73</t>
+  </si>
+  <si>
+    <t>gcc73-lto</t>
+  </si>
+  <si>
+    <t>Intel(R) Atom(TM) CPU  C2750  @ 2.40GHz</t>
+  </si>
+  <si>
+    <t>Intel(R) Core(TM) i5-6287U CPU @ 3.10GHz</t>
   </si>
 </sst>
 </file>
@@ -125,7 +142,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Cost of traversing ten stack frames on x64</a:t>
+              <a:t>Cost of traversing ten stack frames on x64 Intel Skylake</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -142,7 +159,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>'Intel Skylake x64'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -158,7 +175,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>'Intel Skylake x64'!$A$3:$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -187,7 +204,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$9</c:f>
+              <c:f>'Intel Skylake x64'!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -221,7 +238,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>'Intel Skylake x64'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -237,7 +254,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>'Intel Skylake x64'!$A$3:$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -266,7 +283,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$9</c:f>
+              <c:f>'Intel Skylake x64'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -300,7 +317,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>'Intel Skylake x64'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -316,7 +333,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>'Intel Skylake x64'!$A$3:$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -345,7 +362,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$9</c:f>
+              <c:f>'Intel Skylake x64'!$E$3:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -379,7 +396,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>'Intel Skylake x64'!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -398,7 +415,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$9</c:f>
+              <c:f>'Intel Skylake x64'!$H$3:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -432,7 +449,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
+              <c:f>'Intel Skylake x64'!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -451,7 +468,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$9</c:f>
+              <c:f>'Intel Skylake x64'!$I$3:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -485,7 +502,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>'Intel Skylake x64'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -501,7 +518,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$9</c:f>
+              <c:f>'Intel Skylake x64'!$C$3:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -524,24 +541,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="104049664"/>
-        <c:axId val="104362752"/>
+        <c:axId val="169098240"/>
+        <c:axId val="169108224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="104049664"/>
+        <c:axId val="169098240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104362752"/>
+        <c:crossAx val="169108224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104362752"/>
+        <c:axId val="169108224"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -568,7 +585,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104049664"/>
+        <c:crossAx val="169098240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -591,7 +608,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -611,9 +628,10 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Cost of traversing ten stack frames on x64</a:t>
+              <a:rPr lang="en-GB" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>Cost of traversing ten stack frames on x64 Intel Skylake</a:t>
             </a:r>
+            <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -629,7 +647,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>'Intel Skylake x64'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -645,7 +663,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>'Intel Skylake x64'!$A$3:$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -674,7 +692,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$9</c:f>
+              <c:f>'Intel Skylake x64'!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -708,7 +726,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>'Intel Skylake x64'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -724,7 +742,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>'Intel Skylake x64'!$A$3:$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -753,7 +771,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$9</c:f>
+              <c:f>'Intel Skylake x64'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -787,7 +805,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>'Intel Skylake x64'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -803,7 +821,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>'Intel Skylake x64'!$A$3:$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -832,7 +850,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$9</c:f>
+              <c:f>'Intel Skylake x64'!$E$3:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -866,7 +884,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>'Intel Skylake x64'!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -885,7 +903,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$9</c:f>
+              <c:f>'Intel Skylake x64'!$H$3:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -919,7 +937,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
+              <c:f>'Intel Skylake x64'!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -938,7 +956,7 @@
           </c:spPr>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$9</c:f>
+              <c:f>'Intel Skylake x64'!$I$3:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -967,24 +985,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="119894784"/>
-        <c:axId val="184440320"/>
+        <c:axId val="169501056"/>
+        <c:axId val="169502592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="119894784"/>
+        <c:axId val="169501056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184440320"/>
+        <c:crossAx val="169502592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="184440320"/>
+        <c:axId val="169502592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1010,7 +1028,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119894784"/>
+        <c:crossAx val="169501056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1033,7 +1051,787 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Cost of traversing ten stack frames on x64 Intel Silvermont</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Intel Silvermont x64'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>null case</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Intel Silvermont x64'!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gcc73-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gcc73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc73-lto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clang73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Intel Silvermont x64'!$B$3:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>202.61832000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200.898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>235.05912000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150.83496</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Intel Silvermont x64'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>success (error code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Intel Silvermont x64'!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gcc73-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gcc73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc73-lto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clang73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Intel Silvermont x64'!$D$3:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>395.01936000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>406.49856</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>235.17287999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>294.96096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Intel Silvermont x64'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>failure (error code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Intel Silvermont x64'!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gcc73-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gcc73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc73-lto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clang73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Intel Silvermont x64'!$E$3:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>392.7432</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>413.52431999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>235.16087999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>272.62896000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Intel Silvermont x64'!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>success (experimental status code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Intel Silvermont x64'!$H$3:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>291.35784000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>296.57904000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>235.10471999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>175.96152000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Intel Silvermont x64'!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>failure (experimental status code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Intel Silvermont x64'!$I$3:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>291.57119999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>294.79392000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>234.65904</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>185.56344000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Intel Silvermont x64'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>exception throw-catch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Intel Silvermont x64'!$C$3:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="1">
+                  <c:v>160102.72344</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20179.887839999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>154733.89848</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="184032256"/>
+        <c:axId val="184046336"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="184032256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="184046336"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="184046336"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Total CPU cycles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="184032256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>Cost of traversing ten stack frames on x64 Intel Silvermont</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Intel Silvermont x64'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>null case</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Intel Silvermont x64'!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gcc73-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gcc73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc73-lto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clang73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Intel Silvermont x64'!$B$3:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>202.61832000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200.898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>235.05912000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150.83496</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Intel Silvermont x64'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>success (error code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Intel Silvermont x64'!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gcc73-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gcc73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc73-lto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clang73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Intel Silvermont x64'!$D$3:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>395.01936000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>406.49856</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>235.17287999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>294.96096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Intel Silvermont x64'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>failure (error code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Intel Silvermont x64'!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gcc73-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gcc73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc73-lto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clang73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Intel Silvermont x64'!$E$3:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>392.7432</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>413.52431999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>235.16087999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>272.62896000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Intel Silvermont x64'!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>success (experimental status code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Intel Silvermont x64'!$H$3:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>291.35784000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>296.57904000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>235.10471999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>175.96152000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Intel Silvermont x64'!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>failure (experimental status code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'Intel Silvermont x64'!$I$3:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>291.57119999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>294.79392000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>234.65904</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>185.56344000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="184091008"/>
+        <c:axId val="184092544"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="184091008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="184092544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="184092544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Total CPU cycles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="184091008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1045,13 +1843,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>222250</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>342950</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>124250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1075,18 +1873,83 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>41</xdr:col>
       <xdr:colOff>38150</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>130600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>342950</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>124250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>38150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>130600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1389,248 +2252,253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.53125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.06640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>82.424570000000003</v>
-      </c>
-      <c r="D2">
-        <v>81.678510000000003</v>
-      </c>
-      <c r="E2">
-        <v>82.764660000000006</v>
-      </c>
-      <c r="F2">
-        <v>98.672160000000005</v>
-      </c>
-      <c r="G2">
-        <v>96.565849999999998</v>
-      </c>
-      <c r="H2">
-        <v>88.50273</v>
-      </c>
-      <c r="I2">
-        <v>85.55274</v>
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>82.707740000000001</v>
-      </c>
-      <c r="C3">
-        <v>41302.28213</v>
+        <v>82.424570000000003</v>
       </c>
       <c r="D3">
-        <v>88.960840000000005</v>
+        <v>81.678510000000003</v>
       </c>
       <c r="E3">
-        <v>85.397329999999997</v>
+        <v>82.764660000000006</v>
       </c>
       <c r="F3">
-        <v>86.400289999999998</v>
+        <v>98.672160000000005</v>
       </c>
       <c r="G3">
-        <v>481.47708999999998</v>
+        <v>96.565849999999998</v>
       </c>
       <c r="H3">
-        <v>82.794759999999997</v>
+        <v>88.50273</v>
       </c>
       <c r="I3">
-        <v>86.688599999999994</v>
+        <v>85.55274</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>91.374139999999997</v>
+        <v>82.707740000000001</v>
       </c>
       <c r="C4">
-        <v>4605.8144899999998</v>
+        <v>41302.28213</v>
       </c>
       <c r="D4">
-        <v>92.785290000000003</v>
+        <v>88.960840000000005</v>
       </c>
       <c r="E4">
-        <v>91.785889999999995</v>
+        <v>85.397329999999997</v>
       </c>
       <c r="F4">
-        <v>93.126189999999994</v>
+        <v>86.400289999999998</v>
       </c>
       <c r="G4">
-        <v>305.27650999999997</v>
+        <v>481.47708999999998</v>
       </c>
       <c r="H4">
-        <v>87.292519999999996</v>
+        <v>82.794759999999997</v>
       </c>
       <c r="I4">
-        <v>89.312989999999999</v>
+        <v>86.688599999999994</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>91.374139999999997</v>
+      </c>
+      <c r="C5">
+        <v>4605.8144899999998</v>
+      </c>
+      <c r="D5">
+        <v>92.785290000000003</v>
+      </c>
+      <c r="E5">
+        <v>91.785889999999995</v>
+      </c>
+      <c r="F5">
+        <v>93.126189999999994</v>
+      </c>
+      <c r="G5">
+        <v>305.27650999999997</v>
+      </c>
+      <c r="H5">
+        <v>87.292519999999996</v>
+      </c>
+      <c r="I5">
+        <v>89.312989999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>80.194599999999994</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>42709.761350000001</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>83.502340000000004</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>90.926379999999995</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>93.079610000000002</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <v>388.19351</v>
       </c>
-      <c r="H5">
+      <c r="H6">
         <v>86.220759999999999</v>
       </c>
-      <c r="I5">
+      <c r="I6">
         <v>83.911699999999996</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>96.921149999999997</v>
-      </c>
-      <c r="D7">
-        <v>110.91655</v>
-      </c>
-      <c r="E7">
-        <v>129.85785000000001</v>
-      </c>
-      <c r="F7">
-        <v>91.225800000000007</v>
-      </c>
-      <c r="G7">
-        <v>909.75491999999997</v>
-      </c>
-      <c r="H7">
-        <v>87.248260000000002</v>
-      </c>
-      <c r="I7">
-        <v>83.607500000000002</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>82.727720000000005</v>
-      </c>
-      <c r="C8">
-        <v>27334.886299999998</v>
+        <v>96.921149999999997</v>
       </c>
       <c r="D8">
-        <v>122.34922</v>
+        <v>110.91655</v>
       </c>
       <c r="E8">
-        <v>132.70983000000001</v>
+        <v>129.85785000000001</v>
       </c>
       <c r="F8">
-        <v>90.149990000000003</v>
+        <v>91.225800000000007</v>
       </c>
       <c r="G8">
-        <v>1049.1502800000001</v>
+        <v>909.75491999999997</v>
       </c>
       <c r="H8">
-        <v>93.45993</v>
+        <v>87.248260000000002</v>
       </c>
       <c r="I8">
-        <v>87.351600000000005</v>
+        <v>83.607500000000002</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>82.727720000000005</v>
+      </c>
+      <c r="C9">
+        <v>27334.886299999998</v>
+      </c>
+      <c r="D9">
+        <v>122.34922</v>
+      </c>
+      <c r="E9">
+        <v>132.70983000000001</v>
+      </c>
+      <c r="F9">
+        <v>90.149990000000003</v>
+      </c>
+      <c r="G9">
+        <v>1049.1502800000001</v>
+      </c>
+      <c r="H9">
+        <v>93.45993</v>
+      </c>
+      <c r="I9">
+        <v>87.351600000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>96.569659999999999</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>25847.482609999999</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>118.07134000000001</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>85.29853</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>92.844160000000002</v>
       </c>
-      <c r="G9">
+      <c r="G10">
         <v>1017.91062</v>
       </c>
-      <c r="H9">
+      <c r="H10">
         <v>93.096260000000001</v>
       </c>
-      <c r="I9">
+      <c r="I10">
         <v>86.162400000000005</v>
       </c>
     </row>
@@ -1642,24 +2510,174 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="M9" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:I12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.53125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.06640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>202.61832000000001</v>
+      </c>
+      <c r="D3">
+        <v>395.01936000000001</v>
+      </c>
+      <c r="E3">
+        <v>392.7432</v>
+      </c>
+      <c r="F3">
+        <v>463.85255999999998</v>
+      </c>
+      <c r="G3">
+        <v>646.03728000000001</v>
+      </c>
+      <c r="H3">
+        <v>291.35784000000001</v>
+      </c>
+      <c r="I3">
+        <v>291.57119999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>200.898</v>
+      </c>
+      <c r="C4">
+        <v>160102.72344</v>
+      </c>
+      <c r="D4">
+        <v>406.49856</v>
+      </c>
+      <c r="E4">
+        <v>413.52431999999999</v>
+      </c>
+      <c r="F4">
+        <v>457.54608000000002</v>
+      </c>
+      <c r="G4">
+        <v>1174.4203199999999</v>
+      </c>
+      <c r="H4">
+        <v>296.57904000000002</v>
+      </c>
+      <c r="I4">
+        <v>294.79392000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>235.05912000000001</v>
+      </c>
+      <c r="C5">
+        <v>20179.887839999999</v>
+      </c>
+      <c r="D5">
+        <v>235.17287999999999</v>
+      </c>
+      <c r="E5">
+        <v>235.16087999999999</v>
+      </c>
+      <c r="F5">
+        <v>317.00328000000002</v>
+      </c>
+      <c r="G5">
+        <v>1029.2659200000001</v>
+      </c>
+      <c r="H5">
+        <v>235.10471999999999</v>
+      </c>
+      <c r="I5">
+        <v>234.65904</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>150.83496</v>
+      </c>
+      <c r="C6">
+        <v>154733.89848</v>
+      </c>
+      <c r="D6">
+        <v>294.96096</v>
+      </c>
+      <c r="E6">
+        <v>272.62896000000001</v>
+      </c>
+      <c r="F6">
+        <v>362.25936000000002</v>
+      </c>
+      <c r="G6">
+        <v>1041.91416</v>
+      </c>
+      <c r="H6">
+        <v>175.96152000000001</v>
+      </c>
+      <c r="I6">
+        <v>185.56344000000001</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated benchmarks and FAQ with results for Silvermont, ARM Cortex A72 and A53 CPUs.
</commit_message>
<xml_diff>
--- a/benchmark/results.v2.1.xlsx
+++ b/benchmark/results.v2.1.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="113" windowWidth="23168" windowHeight="12503"/>
+    <workbookView xWindow="240" yWindow="113" windowWidth="23168" windowHeight="12503" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Intel Skylake x64" sheetId="1" r:id="rId1"/>
     <sheet name="Intel Silvermont x64" sheetId="4" r:id="rId2"/>
+    <sheet name="ARM64 Cortex A72" sheetId="5" r:id="rId3"/>
+    <sheet name="ARM64 Cortex A53" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="24">
   <si>
     <t>Compiler</t>
   </si>
@@ -81,6 +83,12 @@
   </si>
   <si>
     <t>Intel(R) Core(TM) i5-6287U CPU @ 3.10GHz</t>
+  </si>
+  <si>
+    <t>ARM Cortex A72 @ 2.10GHz</t>
+  </si>
+  <si>
+    <t>ARM Cortex A53 @ 1.70GHz</t>
   </si>
 </sst>
 </file>
@@ -541,24 +549,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="169098240"/>
-        <c:axId val="169108224"/>
+        <c:axId val="188824192"/>
+        <c:axId val="188838272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="169098240"/>
+        <c:axId val="188824192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169108224"/>
+        <c:crossAx val="188838272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="169108224"/>
+        <c:axId val="188838272"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -585,7 +593,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169098240"/>
+        <c:crossAx val="188824192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -608,7 +616,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -635,7 +643,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -985,24 +992,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="169501056"/>
-        <c:axId val="169502592"/>
+        <c:axId val="189026304"/>
+        <c:axId val="189027840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="169501056"/>
+        <c:axId val="189026304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169502592"/>
+        <c:crossAx val="189027840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="169502592"/>
+        <c:axId val="189027840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1024,18 +1031,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169501056"/>
+        <c:crossAx val="189026304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1051,7 +1056,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1393,24 +1398,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="184032256"/>
-        <c:axId val="184046336"/>
+        <c:axId val="189187968"/>
+        <c:axId val="189189504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="184032256"/>
+        <c:axId val="189187968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184046336"/>
+        <c:crossAx val="189189504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="184046336"/>
+        <c:axId val="189189504"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1437,7 +1442,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184032256"/>
+        <c:crossAx val="189187968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1460,7 +1465,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1487,7 +1492,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1765,24 +1769,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="184091008"/>
-        <c:axId val="184092544"/>
+        <c:axId val="189115008"/>
+        <c:axId val="189124992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="184091008"/>
+        <c:axId val="189115008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184092544"/>
+        <c:crossAx val="189124992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="184092544"/>
+        <c:axId val="189124992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1804,11 +1808,423 @@
               </a:p>
             </c:rich>
           </c:tx>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="189115008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Cost of traversing ten stack frames on ARM64</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Cortex A72</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A72'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>null case</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A72'!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gcc73-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gcc73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc73-lto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clang73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A72'!$B$3:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>131.72324</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>132.35857999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>126.14765</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>133.69739000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A72'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>success (error code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A72'!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gcc73-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gcc73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc73-lto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clang73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A72'!$D$3:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>138.23886999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>134.40727999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>126.15736</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>138.21294</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A72'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>failure (error code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A72'!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gcc73-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gcc73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc73-lto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clang73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A72'!$E$3:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>137.39121</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>135.50296</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>132.74755999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>138.30696</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A72'!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>success (experimental status code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A72'!$H$3:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>135.32142999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>144.25857999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>126.1752</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>133.47693000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A72'!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>failure (experimental status code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A72'!$I$3:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>143.30553</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>152.35938999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>133.26948999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128.87223</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A72'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>exception throw-catch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A72'!$C$3:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="1">
+                  <c:v>92120.392850000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9493.2770600000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85594.600120000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="122158080"/>
+        <c:axId val="122172160"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="122158080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="122172160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="122172160"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Total CPU cycles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184091008"/>
+        <c:crossAx val="122158080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1831,7 +2247,1187 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>Cost of traversing ten stack frames on ARM64 Cortex A72</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A72'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>null case</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A72'!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gcc73-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gcc73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc73-lto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clang73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A72'!$B$3:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>131.72324</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>132.35857999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>126.14765</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>133.69739000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A72'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>success (error code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A72'!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gcc73-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gcc73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc73-lto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clang73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A72'!$D$3:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>138.23886999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>134.40727999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>126.15736</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>138.21294</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A72'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>failure (error code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A72'!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gcc73-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gcc73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc73-lto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clang73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A72'!$E$3:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>137.39121</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>135.50296</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>132.74755999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>138.30696</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A72'!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>success (experimental status code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A72'!$H$3:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>135.32142999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>144.25857999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>126.1752</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>133.47693000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A72'!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>failure (experimental status code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A72'!$I$3:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>143.30553</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>152.35938999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>133.26948999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128.87223</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="122237312"/>
+        <c:axId val="122238848"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="122237312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="122238848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="122238848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Total CPU cycles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="122237312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Cost of traversing ten stack frames on ARM64</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Cortex A53</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A53'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>null case</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A53'!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gcc73-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gcc73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc73-lto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clang73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A53'!$B$3:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>189.29107999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>215.29850999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73.094070000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>163.22076000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A53'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>success (error code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A53'!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gcc73-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gcc73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc73-lto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clang73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A53'!$D$3:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>286.63846999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>313.41489000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73.104560000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>188.49327</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A53'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>failure (error code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A53'!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gcc73-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gcc73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc73-lto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clang73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A53'!$E$3:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>289.11831000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>314.62533999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74.100139999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>189.48365000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A53'!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>success (experimental status code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A53'!$H$3:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>276.41131000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>307.7439</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73.101920000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>169.48518000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A53'!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>failure (experimental status code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A53'!$I$3:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>279.41120999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>308.51940999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74.096220000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>175.30288999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A53'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>exception throw-catch</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A53'!$C$3:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="1">
+                  <c:v>153112.21179999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16716.28775</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>145274.39009999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="48170496"/>
+        <c:axId val="48172032"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="48170496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="48172032"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="48172032"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Total CPU cycles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="48170496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="2160" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>Cost of traversing ten stack frames on </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>ARM64 Cortex A53</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A53'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>null case</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="92D050"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A53'!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gcc73-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gcc73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc73-lto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clang73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A53'!$B$3:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>189.29107999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>215.29850999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73.094070000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>163.22076000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A53'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>success (error code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A53'!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gcc73-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gcc73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc73-lto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clang73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A53'!$D$3:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>286.63846999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>313.41489000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73.104560000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>188.49327</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A53'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>failure (error code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A53'!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>gcc73-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gcc73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc73-lto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clang73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A53'!$E$3:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>289.11831000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>314.62533999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74.100139999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>189.48365000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A53'!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>success (experimental status code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A53'!$H$3:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>276.41131000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>307.7439</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73.101920000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>169.48518000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'ARM64 Cortex A53'!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>failure (experimental status code)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'ARM64 Cortex A53'!$I$3:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>279.41120999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>308.51940999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74.096220000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>175.30288999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="48224896"/>
+        <c:axId val="48632192"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="48224896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="48632192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="48632192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Total CPU cycles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="48224896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1903,6 +3499,136 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>342950</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>124250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>38150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>130600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>342950</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>124250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>38150</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>130600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2254,7 +3980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
@@ -2512,8 +4238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView topLeftCell="M9" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2680,4 +4406,348 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.53125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.06640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>131.72324</v>
+      </c>
+      <c r="D3">
+        <v>138.23886999999999</v>
+      </c>
+      <c r="E3">
+        <v>137.39121</v>
+      </c>
+      <c r="F3">
+        <v>140.72682</v>
+      </c>
+      <c r="G3">
+        <v>158.82479000000001</v>
+      </c>
+      <c r="H3">
+        <v>135.32142999999999</v>
+      </c>
+      <c r="I3">
+        <v>143.30553</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>132.35857999999999</v>
+      </c>
+      <c r="C4">
+        <v>92120.392850000004</v>
+      </c>
+      <c r="D4">
+        <v>134.40727999999999</v>
+      </c>
+      <c r="E4">
+        <v>135.50296</v>
+      </c>
+      <c r="F4">
+        <v>153.81811999999999</v>
+      </c>
+      <c r="G4">
+        <v>394.03350999999998</v>
+      </c>
+      <c r="H4">
+        <v>144.25857999999999</v>
+      </c>
+      <c r="I4">
+        <v>152.35938999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>126.14765</v>
+      </c>
+      <c r="C5">
+        <v>9493.2770600000003</v>
+      </c>
+      <c r="D5">
+        <v>126.15736</v>
+      </c>
+      <c r="E5">
+        <v>132.74755999999999</v>
+      </c>
+      <c r="F5">
+        <v>126.1752</v>
+      </c>
+      <c r="G5">
+        <v>328.73917</v>
+      </c>
+      <c r="H5">
+        <v>126.1752</v>
+      </c>
+      <c r="I5">
+        <v>133.26948999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>133.69739000000001</v>
+      </c>
+      <c r="C6">
+        <v>85594.600120000003</v>
+      </c>
+      <c r="D6">
+        <v>138.21294</v>
+      </c>
+      <c r="E6">
+        <v>138.30696</v>
+      </c>
+      <c r="F6">
+        <v>133.34565000000001</v>
+      </c>
+      <c r="G6">
+        <v>394.81635</v>
+      </c>
+      <c r="H6">
+        <v>133.47693000000001</v>
+      </c>
+      <c r="I6">
+        <v>128.87223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.53125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.06640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>189.29107999999999</v>
+      </c>
+      <c r="D3">
+        <v>286.63846999999998</v>
+      </c>
+      <c r="E3">
+        <v>289.11831000000001</v>
+      </c>
+      <c r="F3">
+        <v>310.56693000000001</v>
+      </c>
+      <c r="G3">
+        <v>355.47505999999998</v>
+      </c>
+      <c r="H3">
+        <v>276.41131000000001</v>
+      </c>
+      <c r="I3">
+        <v>279.41120999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>215.29850999999999</v>
+      </c>
+      <c r="C4">
+        <v>153112.21179999999</v>
+      </c>
+      <c r="D4">
+        <v>313.41489000000001</v>
+      </c>
+      <c r="E4">
+        <v>314.62533999999999</v>
+      </c>
+      <c r="F4">
+        <v>341.96503000000001</v>
+      </c>
+      <c r="G4">
+        <v>698.20119</v>
+      </c>
+      <c r="H4">
+        <v>307.7439</v>
+      </c>
+      <c r="I4">
+        <v>308.51940999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>73.094070000000002</v>
+      </c>
+      <c r="C5">
+        <v>16716.28775</v>
+      </c>
+      <c r="D5">
+        <v>73.104560000000006</v>
+      </c>
+      <c r="E5">
+        <v>74.100139999999996</v>
+      </c>
+      <c r="F5">
+        <v>86.439030000000002</v>
+      </c>
+      <c r="G5">
+        <v>422.81691000000001</v>
+      </c>
+      <c r="H5">
+        <v>73.101920000000007</v>
+      </c>
+      <c r="I5">
+        <v>74.096220000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>163.22076000000001</v>
+      </c>
+      <c r="C6">
+        <v>145274.39009999999</v>
+      </c>
+      <c r="D6">
+        <v>188.49327</v>
+      </c>
+      <c r="E6">
+        <v>189.48365000000001</v>
+      </c>
+      <c r="F6">
+        <v>192.64336</v>
+      </c>
+      <c r="G6">
+        <v>544.21722</v>
+      </c>
+      <c r="H6">
+        <v>169.48518000000001</v>
+      </c>
+      <c r="I6">
+        <v>175.30288999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>